<commit_message>
sending message?? have not deleted other strategies
</commit_message>
<xml_diff>
--- a/SampleInventory.xlsx
+++ b/SampleInventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cs_projects\SCBC_SnackShackServer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6AD32E2-759B-4028-A75B-BD14CA1BA7A8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AF10F2-32CB-41BA-A102-2F074B94AF6B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="528" yWindow="3144" windowWidth="17280" windowHeight="8964" xr2:uid="{55BEEBE3-4AC0-4972-A6F9-8725157C82F2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -145,14 +145,16 @@
   </si>
   <si>
     <t>Zach's Croc</t>
+  </si>
+  <si>
+    <t>Nathan's Eye Bags (Unwashed)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
@@ -201,13 +203,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -523,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B237B8BA-060B-482C-829A-F030DEA8E613}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,7 +608,7 @@
       <c r="B7">
         <v>15</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>12</v>
       </c>
     </row>
@@ -640,7 +641,7 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="3">
         <v>200</v>
       </c>
     </row>
@@ -662,8 +663,8 @@
       <c r="B12">
         <v>300</v>
       </c>
-      <c r="C12" s="5">
-        <v>500</v>
+      <c r="C12" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -675,6 +676,17 @@
       </c>
       <c r="C13" s="3">
         <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>